<commit_message>
Conversa sobre a heuristica 2
</commit_message>
<xml_diff>
--- a/Estatísticas.xlsx
+++ b/Estatísticas.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="13">
   <si>
     <t>algoritmo</t>
   </si>
@@ -61,64 +61,13 @@
     <t>tempo (seg)</t>
   </si>
   <si>
-    <t>0.0689</t>
-  </si>
-  <si>
-    <t>4.8144</t>
-  </si>
-  <si>
-    <t>0.0013</t>
-  </si>
-  <si>
-    <t>38.6835</t>
-  </si>
-  <si>
     <t>Profundidade máxima</t>
   </si>
   <si>
-    <t>0.0520</t>
-  </si>
-  <si>
-    <t>2.2148</t>
-  </si>
-  <si>
-    <t>0.0277</t>
-  </si>
-  <si>
-    <t>7.9453</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.0023</t>
-  </si>
-  <si>
-    <t>439.1406</t>
-  </si>
-  <si>
     <t>fator de ramificação (margem 0.5 erro)</t>
   </si>
   <si>
-    <t>0.025</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>38.75</t>
-  </si>
-  <si>
     <t>indefinido</t>
-  </si>
-  <si>
-    <t>0.0272</t>
-  </si>
-  <si>
-    <t>1.5190</t>
-  </si>
-  <si>
-    <t>6.9886e-6</t>
   </si>
 </sst>
 </file>
@@ -477,7 +426,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,105 +460,31 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1536</v>
-      </c>
-      <c r="D2">
-        <v>64</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>96</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>29</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>72</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -618,6 +493,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -657,193 +606,30 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>440</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>40</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>440</v>
-      </c>
-      <c r="D3">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1144711</v>
-      </c>
-      <c r="D4">
-        <v>343</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -885,10 +671,10 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -947,10 +733,10 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1009,10 +795,10 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Separação do código em 3 ficheiros Formatação do código da heuristica 2
</commit_message>
<xml_diff>
--- a/Estatísticas.xlsx
+++ b/Estatísticas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tabuleiro A" sheetId="1" r:id="rId1"/>
@@ -5922,16 +5922,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6303,7 +6303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -6451,7 +6451,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6519,6 +6519,9 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -6577,7 +6580,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6813,138 +6816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>770</v>
-      </c>
-      <c r="D3">
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>536</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-      <c r="E4">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>602</v>
-      </c>
-      <c r="D5">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -6998,6 +6870,137 @@
         <v>3</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>770</v>
+      </c>
+      <c r="D3">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>536</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>602</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">

</xml_diff>